<commit_message>
[pascal] Pascal laba #6 - Trees
</commit_message>
<xml_diff>
--- a/pascal/list_labels.xlsx
+++ b/pascal/list_labels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Чебураш</t>
   </si>
@@ -74,19 +74,7 @@
     <t>Время</t>
   </si>
   <si>
-    <t>И-212</t>
-  </si>
-  <si>
-    <t>13:30 - 14:50</t>
-  </si>
-  <si>
-    <t>08:20 - 09:40</t>
-  </si>
-  <si>
-    <t>15:00 - 16:20</t>
-  </si>
-  <si>
-    <t>09:50 - 11:10</t>
+    <t>~</t>
   </si>
 </sst>
 </file>
@@ -435,7 +423,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,15 +459,9 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3">
-        <v>44945</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -490,23 +472,18 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
-        <v>44946</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -514,9 +491,7 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
[pascal] Laba #10 - O zagruzke
</commit_message>
<xml_diff>
--- a/pascal/list_labels.xlsx
+++ b/pascal/list_labels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Чебураш</t>
   </si>
@@ -423,7 +423,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,6 +523,9 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">

</xml_diff>